<commit_message>
CCRU KPI template fix
</commit_message>
<xml_diff>
--- a/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub - REG.xlsx
+++ b/Projects/CCRU/Data/KPIs_2019/PoS 2019 - IC HoReCa BarTavernClub - REG.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\New folder (160)\INTEGR\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFE6D70F-0FF3-4476-998C-DEC44A467B71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10725" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="HoReCa Bar Tavern_Night Club" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AM$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AM$49</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'HoReCa Bar Tavern_Night Club'!$A$1:$AM$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">'HoReCa Bar Tavern_Night Club'!$A$1:$AM$48</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">'HoReCa Bar Tavern_Night Club'!$A$1:$AM$48</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -25,138 +30,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="213">
-  <si>
-    <t xml:space="preserve">Sorting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP PoS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP KPI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI name Eng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI name Rus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Result Format</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Target</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">target_max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Values</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacturer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logical Operator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Form Factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Products to exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zone to include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locations to exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Locations to include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenes to include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenes to exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub locations to include</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sub locations to exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score_func</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI Weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score_min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">score_max</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">level</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Children</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RD38000024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HoReCa_Bar_Tavern_Night_Clubs_REG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Представленность</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="214">
+  <si>
+    <t>Sorting</t>
+  </si>
+  <si>
+    <t>SAP PoS</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>KPI Type</t>
+  </si>
+  <si>
+    <t>SAP KPI</t>
+  </si>
+  <si>
+    <t>KPI name Eng</t>
+  </si>
+  <si>
+    <t>KPI name Rus</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Result Format</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>target_min</t>
+  </si>
+  <si>
+    <t>target_max</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Values</t>
+  </si>
+  <si>
+    <t>Product Category</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Sub category</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Logical Operator</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Form Factor</t>
+  </si>
+  <si>
+    <t>Products to exclude</t>
+  </si>
+  <si>
+    <t>Zone to include</t>
+  </si>
+  <si>
+    <t>Locations to exclude</t>
+  </si>
+  <si>
+    <t>Locations to include</t>
+  </si>
+  <si>
+    <t>Scenes to include</t>
+  </si>
+  <si>
+    <t>Scenes to exclude</t>
+  </si>
+  <si>
+    <t>sub locations to include</t>
+  </si>
+  <si>
+    <t>sub locations to exclude</t>
+  </si>
+  <si>
+    <t>score_func</t>
+  </si>
+  <si>
+    <t>KPI Weight</t>
+  </si>
+  <si>
+    <t>score_min</t>
+  </si>
+  <si>
+    <t>score_max</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>level</t>
+  </si>
+  <si>
+    <t>KPI ID</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>RD38000024</t>
+  </si>
+  <si>
+    <t>HoReCa_Bar_Tavern_Night_Clubs_REG</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Представленность</t>
   </si>
   <si>
     <t xml:space="preserve">1
@@ -166,26 +171,26 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Coolers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Холодильники</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311
+    <t>Coolers</t>
+  </si>
+  <si>
+    <t>Холодильники</t>
+  </si>
+  <si>
+    <t>311
 312</t>
   </si>
   <si>
-    <t xml:space="preserve">Coolers: Quality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Холодильник: Качество</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активации</t>
+    <t>Coolers: Quality</t>
+  </si>
+  <si>
+    <t>Холодильник: Качество</t>
+  </si>
+  <si>
+    <t>Activations</t>
+  </si>
+  <si>
+    <t>Активации</t>
   </si>
   <si>
     <t xml:space="preserve">23
@@ -194,16 +199,16 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">STANDARD 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Представленность SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Weighted Average</t>
+    <t>STANDARD 1</t>
+  </si>
+  <si>
+    <t>SSD Availability</t>
+  </si>
+  <si>
+    <t>Представленность SSD</t>
+  </si>
+  <si>
+    <t>Weighted Average</t>
   </si>
   <si>
     <t xml:space="preserve">Weighted Average </t>
@@ -219,124 +224,124 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Coca-Cola - 0.33L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола - 0.33л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of facings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SKUs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panoramic Photo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BINARY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Tonic - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Тоник - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola Zero - 0.33L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Кока-Кола Зеро - 0.33л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Bitter Lemon - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Биттер Лемон - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Aperol Spritz - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Шпритц - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schweppes Ginger Spritz - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Швеппс Имбирь - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.25L Glass/Fanta Orange - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Спрайт - 0.25л стекло/ Фанта Апельсин - 0.25л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprite - 0.25L Glass, Fanta Orange - 0.25L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54490970, 40822419, 87126860, 50112135</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STANDARD 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Представленность Воды</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 0.33L Glass/ BonAqua Carb - 0.33L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">БонАква Негаз - 0.33л стекло/БонАква Газ - 0.33л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BonAqua Still - 0.33L Glass, BonAqua Carb - 0.33L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90418822, 90382741</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juice Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Представленность Сока</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12
+    <t>Coca-Cola - 0.33L Glass</t>
+  </si>
+  <si>
+    <t>Кока-Кола - 0.33л стекло</t>
+  </si>
+  <si>
+    <t>number of facings</t>
+  </si>
+  <si>
+    <t>OR</t>
+  </si>
+  <si>
+    <t>SKUs</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Panoramic Photo</t>
+  </si>
+  <si>
+    <t>BINARY</t>
+  </si>
+  <si>
+    <t>Schweppes Tonic - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>Швеппс Тоник - 0.25л стекло</t>
+  </si>
+  <si>
+    <t>Coca-Cola Zero - 0.33L Glass</t>
+  </si>
+  <si>
+    <t>Кока-Кола Зеро - 0.33л стекло</t>
+  </si>
+  <si>
+    <t>Schweppes Bitter Lemon - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>Швеппс Биттер Лемон - 0.25л стекло</t>
+  </si>
+  <si>
+    <t>Schweppes Aperol Spritz - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>Швеппс Шпритц - 0.25л стекло</t>
+  </si>
+  <si>
+    <t>Schweppes Ginger Spritz - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>Швеппс Имбирь - 0.25л стекло</t>
+  </si>
+  <si>
+    <t>Sprite - 0.25L Glass/Fanta Orange - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>Спрайт - 0.25л стекло/ Фанта Апельсин - 0.25л стекло</t>
+  </si>
+  <si>
+    <t>Sprite - 0.25L Glass, Fanta Orange - 0.25L Glass</t>
+  </si>
+  <si>
+    <t>54490970, 40822419, 87126860, 50112135</t>
+  </si>
+  <si>
+    <t>STANDARD 2</t>
+  </si>
+  <si>
+    <t>Water Availability</t>
+  </si>
+  <si>
+    <t>Представленность Воды</t>
+  </si>
+  <si>
+    <t>BonAqua Still - 0.33L Glass/ BonAqua Carb - 0.33L Glass</t>
+  </si>
+  <si>
+    <t>БонАква Негаз - 0.33л стекло/БонАква Газ - 0.33л стекло</t>
+  </si>
+  <si>
+    <t>BonAqua Still - 0.33L Glass, BonAqua Carb - 0.33L Glass</t>
+  </si>
+  <si>
+    <t>90418822, 90382741</t>
+  </si>
+  <si>
+    <t>Juice Availability</t>
+  </si>
+  <si>
+    <t>Представленность Сока</t>
+  </si>
+  <si>
+    <t>12
 13
 14
 19</t>
   </si>
   <si>
-    <t xml:space="preserve">Rich - Apple - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Яблоко - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich - Orange - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Апельсин - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich 0.2L Glass other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич 0.2л стекло остальные</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of sub atomic KPI Passed</t>
+    <t>Rich - Apple - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Яблоко - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich - Orange - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Апельсин - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich 0.2L Glass other</t>
+  </si>
+  <si>
+    <t>Рич 0.2л стекло остальные</t>
+  </si>
+  <si>
+    <t>number of sub atomic KPI Passed</t>
   </si>
   <si>
     <t xml:space="preserve">15
@@ -346,121 +351,121 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Rich - Pineapple - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Ананас - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich - Peach - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Персик - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich - Grapefruit - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Грейпфрут - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich - Tomato - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Томат - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rich - Cherry - 0.2L Glass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Рич - Вишня - 0.2л стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Energy Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Представленность Энергетиков</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn/Monster 0.33L/0.5L any</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Берн/Монстер 0.33л/0.5л любой</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Burn, Monster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TCCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRAND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.33, 0.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STANDARD 16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menu Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Меню</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle, Cc Graphic, Cc Glass Graphic, Cc Glass And Bottle, CC Hands, Cc Bottle Graphic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004, 68943577005, 68943577006, 68943577007, 68943577008, 68943577009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Menu Activation, Menu, Menu Insert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STANDARD 17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impulse Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Импульсной зоны</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of atomic KPI Passed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bar Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Impulse: SSD/Water/Juice NRGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Импульс: SSD/Water/Juice Стекло</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manufacture: TCCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SSD, Water, Juices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">glass, GLASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Стола</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Table Activation</t>
+    <t>Rich - Pineapple - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Ананас - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich - Peach - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Персик - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich - Grapefruit - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Грейпфрут - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich - Tomato - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Томат - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Rich - Cherry - 0.2L Glass</t>
+  </si>
+  <si>
+    <t>Рич - Вишня - 0.2л стекло</t>
+  </si>
+  <si>
+    <t>Energy Availability</t>
+  </si>
+  <si>
+    <t>Представленность Энергетиков</t>
+  </si>
+  <si>
+    <t>Burn/Monster 0.33L/0.5L any</t>
+  </si>
+  <si>
+    <t>Берн/Монстер 0.33л/0.5л любой</t>
+  </si>
+  <si>
+    <t>Burn, Monster</t>
+  </si>
+  <si>
+    <t>TCCC</t>
+  </si>
+  <si>
+    <t>BRAND</t>
+  </si>
+  <si>
+    <t>0.33, 0.5</t>
+  </si>
+  <si>
+    <t>STANDARD 16</t>
+  </si>
+  <si>
+    <t>Menu Activation</t>
+  </si>
+  <si>
+    <t>Активация Меню</t>
+  </si>
+  <si>
+    <t>Coca Cola Can, Coca Cola Zero Can 0.33, Coca Cola Zero Bottle, Coca Cola Zero Bottle NRGB, Coca Cola Glass, Coca Cola Cup, Coca Cola Bottle NRGB, Coca Cola Bottle, Cc Graphic, Cc Glass Graphic, Cc Glass And Bottle, CC Hands, Cc Bottle Graphic</t>
+  </si>
+  <si>
+    <t>5050570, 50111114, 50111112, 50111111, 5000006, 5000101, 5000005, 5000004, 68943577005, 68943577006, 68943577007, 68943577008, 68943577009</t>
+  </si>
+  <si>
+    <t>Activation</t>
+  </si>
+  <si>
+    <t>Other Menu Activation, Menu, Menu Insert</t>
+  </si>
+  <si>
+    <t>STANDARD 17</t>
+  </si>
+  <si>
+    <t>Impulse Activation</t>
+  </si>
+  <si>
+    <t>Активация Импульсной зоны</t>
+  </si>
+  <si>
+    <t>number of atomic KPI Passed</t>
+  </si>
+  <si>
+    <t>Bar Activation</t>
+  </si>
+  <si>
+    <t>Impulse: SSD/Water/Juice NRGB</t>
+  </si>
+  <si>
+    <t>Импульс: SSD/Water/Juice Стекло</t>
+  </si>
+  <si>
+    <t>Manufacture: TCCC</t>
+  </si>
+  <si>
+    <t>SSD, Water, Juices</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>glass, GLASS</t>
+  </si>
+  <si>
+    <t>Destination Activation</t>
+  </si>
+  <si>
+    <t>Активация Стола</t>
+  </si>
+  <si>
+    <t>Table Activation</t>
   </si>
   <si>
     <t xml:space="preserve">26
@@ -468,93 +473,93 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Destination: Images</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Стола: Имиджи</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IC Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Destination: Coca-Cola/Bon Aqua NRGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Активация Стола: Coca-Cola/Bon Aqua NRGB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola, Bonaqua</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Local 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any Other Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Другие активации</t>
-  </si>
-  <si>
-    <t xml:space="preserve">900
+    <t>Destination: Images</t>
+  </si>
+  <si>
+    <t>Активация Стола: Имиджи</t>
+  </si>
+  <si>
+    <t>IC Activation</t>
+  </si>
+  <si>
+    <t>Destination: Coca-Cola/Bon Aqua NRGB</t>
+  </si>
+  <si>
+    <t>Активация Стола: Coca-Cola/Bon Aqua NRGB</t>
+  </si>
+  <si>
+    <t>Coca-Cola, Bonaqua</t>
+  </si>
+  <si>
+    <t>Local 21</t>
+  </si>
+  <si>
+    <t>Any Other Activation</t>
+  </si>
+  <si>
+    <t>Другие активации</t>
+  </si>
+  <si>
+    <t>900
 901</t>
   </si>
   <si>
-    <t xml:space="preserve">Local</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any Other Activation: NRGB/Mix</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Другие активации: Cтекло/Миксабилити</t>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Any Other Activation: NRGB/Mix</t>
+  </si>
+  <si>
+    <t>Другие активации: Cтекло/Миксабилити</t>
   </si>
   <si>
     <t xml:space="preserve">Bonaqua, Sprite, Rich, Dobriy, Fanta </t>
   </si>
   <si>
-    <t xml:space="preserve">Mixability, Glass, Mocktails</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any Other Activation: Coca-Cola/food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Другие активации: Кола+ЕДА</t>
-  </si>
-  <si>
-    <t xml:space="preserve">902
+    <t>Mixability, Glass, Mocktails</t>
+  </si>
+  <si>
+    <t>Menu, Menu Insert, Other Menu Activation, Table Activation, Bar Activation</t>
+  </si>
+  <si>
+    <t>Any Other Activation: Coca-Cola/food</t>
+  </si>
+  <si>
+    <t>Другие активации: Кола+ЕДА</t>
+  </si>
+  <si>
+    <t>902
 903</t>
   </si>
   <si>
-    <t xml:space="preserve">Any Other Activation: Coca-Cola/food: Coca-Cola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Другие активации: Кола+ЕДА : Кола</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coca-Cola</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any Other Activation: Coca-Cola/food: Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Другие активации: Кола+ЕДА : Еда</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LOCAL 11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visible Cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Видимый ХО</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler</t>
+    <t>Any Other Activation: Coca-Cola/food: Coca-Cola</t>
+  </si>
+  <si>
+    <t>Другие активации: Кола+ЕДА : Кола</t>
+  </si>
+  <si>
+    <t>Coca-Cola</t>
+  </si>
+  <si>
+    <t>Any Other Activation: Coca-Cola/food: Food</t>
+  </si>
+  <si>
+    <t>Другие активации: Кола+ЕДА : Еда</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>LOCAL 11</t>
+  </si>
+  <si>
+    <t>Visible Cooler</t>
+  </si>
+  <si>
+    <t>Видимый ХО</t>
+  </si>
+  <si>
+    <t>Cooler</t>
   </si>
   <si>
     <t xml:space="preserve">34
@@ -563,188 +568,170 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Cooler is Visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ХО виден</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scenes with no tagging</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCENES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panoramic photo of Cooler</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler fullness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ХО Заполнен</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of filled Coolers (scenes)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOS with empty more than 80%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cooler wo other products</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ХО без посторонней продукции</t>
-  </si>
-  <si>
-    <t xml:space="preserve">number of pure Coolers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Share of TCCC product at least 98%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hidden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIS_COOLER_SAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Visible cooler SAP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KPI result</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decimal.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SESSION LEVEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH_PROD_MENU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCH products present in Customer's menu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Passed or Failed Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MenuC1
+    <t>Cooler is Visible</t>
+  </si>
+  <si>
+    <t>ХО виден</t>
+  </si>
+  <si>
+    <t>Scenes with no tagging</t>
+  </si>
+  <si>
+    <t>SCENES</t>
+  </si>
+  <si>
+    <t>Panoramic photo of Cooler</t>
+  </si>
+  <si>
+    <t>Cooler fullness</t>
+  </si>
+  <si>
+    <t>ХО Заполнен</t>
+  </si>
+  <si>
+    <t>number of filled Coolers (scenes)</t>
+  </si>
+  <si>
+    <t>MAN</t>
+  </si>
+  <si>
+    <t>SOS with empty more than 80%</t>
+  </si>
+  <si>
+    <t>Cooler wo other products</t>
+  </si>
+  <si>
+    <t>ХО без посторонней продукции</t>
+  </si>
+  <si>
+    <t>number of pure Coolers</t>
+  </si>
+  <si>
+    <t>Share of TCCC product at least 98%</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>VIS_COOLER_SAP</t>
+  </si>
+  <si>
+    <t>Visible cooler SAP</t>
+  </si>
+  <si>
+    <t>Decimal.2</t>
+  </si>
+  <si>
+    <t>SESSION LEVEL</t>
+  </si>
+  <si>
+    <t>CCH_PROD_MENU</t>
+  </si>
+  <si>
+    <t>CCH products present in Customer's menu</t>
+  </si>
+  <si>
+    <t>Passed or Failed Value</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>MenuC1
 No_MenuC1</t>
   </si>
   <si>
-    <t xml:space="preserve">ACTIVATION_SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of CCH activation points in SSD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IMPU
+    <t>ACTIVATION_SSD</t>
+  </si>
+  <si>
+    <t>Number of CCH activation points in SSD</t>
+  </si>
+  <si>
+    <t>IMPU
 No_IMPU</t>
   </si>
   <si>
-    <t xml:space="preserve">DEST
+    <t>DEST
 No_DEST</t>
   </si>
   <si>
-    <t xml:space="preserve">LOCAL 21</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACTIVATION_OTHER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANY OTHER ACTIVATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO_MidSoc
-No_DO_MidSoc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EO_forLu
+    <t>ACTIVATION_OTHER</t>
+  </si>
+  <si>
+    <t>ANY OTHER ACTIVATION</t>
+  </si>
+  <si>
+    <t>EO_forLu
 No_EO_forLu</t>
   </si>
   <si>
-    <t xml:space="preserve">OCCASIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRIORITY_OCC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of Priority Occasions activated in the outlet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EO
-No_EO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22
+    <t>OCCASIONS</t>
+  </si>
+  <si>
+    <t>PRIORITY_OCC</t>
+  </si>
+  <si>
+    <t>Number of Priority Occasions activated in the outlet</t>
+  </si>
+  <si>
+    <t>PLAN</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>LOCAL 6</t>
+  </si>
+  <si>
+    <t>sum of atomic scores</t>
+  </si>
+  <si>
+    <t>34
+35
+36</t>
+  </si>
+  <si>
+    <t>local 21</t>
+  </si>
+  <si>
+    <t>SEND VALUE if one KPI from lis is Passed , other No_O_A</t>
+  </si>
+  <si>
+    <t>EO
+No_O_A</t>
+  </si>
+  <si>
+    <t>22
+23
 25
-29
-32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DO
-No_DO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38
-23
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PLAN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Integer</t>
+29</t>
+  </si>
+  <si>
+    <t>DO
+No_O_A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="10">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000000\ _₽_-;\-* #,##0.0000000\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="0.00"/>
-    <numFmt numFmtId="169" formatCode="0%"/>
-    <numFmt numFmtId="170" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
-    <numFmt numFmtId="172" formatCode="@"/>
-    <numFmt numFmtId="173" formatCode="#,##0.0000000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000000\ _₽_-;\-* #,##0.0000000\ _₽_-;_-* \-??\ _₽_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -754,7 +741,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -772,8 +759,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -798,182 +792,153 @@
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="32">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="30">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="173" fontId="7" fillId="0" borderId="1" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1032,72 +997,376 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="1:50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AMK49"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="AC1" activeCellId="0" sqref="AC1"/>
-      <selection pane="bottomLeft" activeCell="AC50" activeCellId="0" sqref="50:50"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="Z1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="AC1" sqref="AC1"/>
+      <selection pane="bottomLeft" activeCell="F42" sqref="F42:AM49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="22.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.9348837209302"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.1674418604651"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.0418604651163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.5209302325581"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="53.9023255813954"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="58.5767441860465"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="32.7348837209302"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="19.2"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8279069767442"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.6279069767442"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="16.1209302325581"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="239.111627906977"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="146.567441860465"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="23.0139534883721"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="18.706976744186"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="27.4418604651163"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="36.0558139534884"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="22.0279069767442"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="15.753488372093"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="9.35348837209302"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="25.2279069767442"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="20.4279069767442"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="26.0883720930233"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="25.5953488372093"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="1" width="71.9906976744186"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="1" width="23.3813953488372"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="1" width="29.2883720930233"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="1" width="29.7813953488372"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="1" width="18.8279069767442"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="1" width="16.9813953488372"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="1" width="14.7674418604651"/>
-    <col collapsed="false" hidden="false" max="34" min="34" style="1" width="15.2604651162791"/>
-    <col collapsed="false" hidden="false" max="35" min="35" style="1" width="34.7023255813953"/>
-    <col collapsed="false" hidden="false" max="36" min="36" style="1" width="9.22790697674419"/>
-    <col collapsed="false" hidden="false" max="37" min="37" style="1" width="10.4604651162791"/>
-    <col collapsed="false" hidden="false" max="38" min="38" style="1" width="12.6744186046512"/>
-    <col collapsed="false" hidden="false" max="1025" min="39" style="1" width="11.0744186046512"/>
+    <col min="1" max="1" width="11.875" style="1"/>
+    <col min="2" max="2" width="13.125" style="1"/>
+    <col min="3" max="3" width="37" style="1"/>
+    <col min="4" max="4" width="13" style="1"/>
+    <col min="5" max="5" width="14.5" style="1"/>
+    <col min="6" max="6" width="53.875" style="1"/>
+    <col min="7" max="7" width="58.625" style="1"/>
+    <col min="8" max="8" width="32.75" style="1"/>
+    <col min="9" max="9" width="19.25" style="1"/>
+    <col min="10" max="10" width="10.875" style="1"/>
+    <col min="11" max="11" width="15.625" style="1"/>
+    <col min="12" max="12" width="16.125" style="1"/>
+    <col min="13" max="13" width="239.125" style="1"/>
+    <col min="14" max="14" width="146.625" style="1"/>
+    <col min="15" max="15" width="23" style="1"/>
+    <col min="16" max="16" width="18.75" style="1"/>
+    <col min="17" max="17" width="27.5" style="1"/>
+    <col min="18" max="18" width="36" style="1"/>
+    <col min="19" max="19" width="22" style="1"/>
+    <col min="20" max="20" width="15.75" style="1"/>
+    <col min="21" max="21" width="9.375" style="1"/>
+    <col min="22" max="22" width="17" style="1"/>
+    <col min="23" max="23" width="25.25" style="1"/>
+    <col min="24" max="24" width="20.375" style="1"/>
+    <col min="25" max="25" width="26.125" style="1"/>
+    <col min="26" max="26" width="25.625" style="1"/>
+    <col min="27" max="27" width="72" style="1"/>
+    <col min="28" max="28" width="23.375" style="1"/>
+    <col min="29" max="29" width="29.25" style="1"/>
+    <col min="30" max="30" width="29.75" style="1"/>
+    <col min="31" max="31" width="18.875" style="1"/>
+    <col min="32" max="32" width="17" style="1"/>
+    <col min="33" max="33" width="14.75" style="1"/>
+    <col min="34" max="34" width="15.25" style="1"/>
+    <col min="35" max="35" width="34.75" style="1"/>
+    <col min="36" max="36" width="9.25" style="1"/>
+    <col min="37" max="37" width="10.5" style="1"/>
+    <col min="38" max="38" width="12.625" style="1"/>
+    <col min="39" max="1025" width="11.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1216,8 +1485,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+    <row r="2" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
         <v>45</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1266,10 +1535,10 @@
       <c r="AG2" s="7"/>
       <c r="AH2" s="7"/>
       <c r="AI2" s="7"/>
-      <c r="AJ2" s="10" t="n">
+      <c r="AJ2" s="10">
         <v>1</v>
       </c>
-      <c r="AK2" s="10" t="n">
+      <c r="AK2" s="10">
         <v>300</v>
       </c>
       <c r="AL2" s="11" t="s">
@@ -1277,8 +1546,8 @@
       </c>
       <c r="AM2" s="7"/>
     </row>
-    <row r="3" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="n">
+    <row r="3" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
         <v>46</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1327,10 +1596,10 @@
       <c r="AG3" s="7"/>
       <c r="AH3" s="7"/>
       <c r="AI3" s="7"/>
-      <c r="AJ3" s="10" t="n">
+      <c r="AJ3" s="10">
         <v>1</v>
       </c>
-      <c r="AK3" s="10" t="n">
+      <c r="AK3" s="10">
         <v>310</v>
       </c>
       <c r="AL3" s="11" t="s">
@@ -1338,8 +1607,8 @@
       </c>
       <c r="AM3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="n">
+    <row r="4" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
         <v>47</v>
       </c>
       <c r="B4" s="7" t="s">
@@ -1388,21 +1657,21 @@
       <c r="AG4" s="7"/>
       <c r="AH4" s="7"/>
       <c r="AI4" s="7"/>
-      <c r="AJ4" s="10" t="n">
+      <c r="AJ4" s="10">
         <v>1</v>
       </c>
-      <c r="AK4" s="10" t="n">
+      <c r="AK4" s="10">
         <v>312</v>
       </c>
-      <c r="AL4" s="7" t="n">
+      <c r="AL4" s="7">
         <v>33</v>
       </c>
-      <c r="AM4" s="10" t="n">
+      <c r="AM4" s="10">
         <v>310</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+    <row r="5" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
         <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -1451,10 +1720,10 @@
       <c r="AG5" s="7"/>
       <c r="AH5" s="7"/>
       <c r="AI5" s="7"/>
-      <c r="AJ5" s="10" t="n">
+      <c r="AJ5" s="10">
         <v>1</v>
       </c>
-      <c r="AK5" s="10" t="n">
+      <c r="AK5" s="10">
         <v>400</v>
       </c>
       <c r="AL5" s="11" t="s">
@@ -1462,8 +1731,8 @@
       </c>
       <c r="AM5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+    <row r="6" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -1516,21 +1785,21 @@
       <c r="AG6" s="7"/>
       <c r="AH6" s="7"/>
       <c r="AI6" s="7"/>
-      <c r="AJ6" s="7" t="n">
+      <c r="AJ6" s="7">
         <v>2</v>
       </c>
-      <c r="AK6" s="7" t="n">
+      <c r="AK6" s="7">
         <v>1</v>
       </c>
       <c r="AL6" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="AM6" s="13" t="n">
+      <c r="AM6" s="13">
         <v>300</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+    <row r="7" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1555,7 +1824,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="7"/>
-      <c r="J7" s="7" t="n">
+      <c r="J7" s="7">
         <v>1</v>
       </c>
       <c r="K7" s="7"/>
@@ -1563,7 +1832,7 @@
       <c r="M7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="N7" s="10" t="n">
+      <c r="N7" s="10">
         <v>50112128</v>
       </c>
       <c r="O7" s="10"/>
@@ -1593,25 +1862,25 @@
       <c r="AE7" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF7" s="9" t="n">
+      <c r="AF7" s="9">
         <v>0.05</v>
       </c>
       <c r="AG7" s="7"/>
       <c r="AH7" s="7"/>
       <c r="AI7" s="7"/>
-      <c r="AJ7" s="7" t="n">
+      <c r="AJ7" s="7">
         <v>3</v>
       </c>
-      <c r="AK7" s="7" t="n">
+      <c r="AK7" s="7">
         <v>2</v>
       </c>
       <c r="AL7" s="7"/>
-      <c r="AM7" s="7" t="n">
+      <c r="AM7" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+    <row r="8" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1636,7 +1905,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="7"/>
-      <c r="J8" s="7" t="n">
+      <c r="J8" s="7">
         <v>1</v>
       </c>
       <c r="K8" s="7"/>
@@ -1644,7 +1913,7 @@
       <c r="M8" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="N8" s="10" t="n">
+      <c r="N8" s="10">
         <v>40822341</v>
       </c>
       <c r="O8" s="10"/>
@@ -1674,25 +1943,25 @@
       <c r="AE8" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF8" s="9" t="n">
+      <c r="AF8" s="9">
         <v>0.05</v>
       </c>
       <c r="AG8" s="7"/>
       <c r="AH8" s="7"/>
       <c r="AI8" s="7"/>
-      <c r="AJ8" s="7" t="n">
+      <c r="AJ8" s="7">
         <v>3</v>
       </c>
-      <c r="AK8" s="7" t="n">
+      <c r="AK8" s="7">
         <v>3</v>
       </c>
       <c r="AL8" s="7"/>
-      <c r="AM8" s="7" t="n">
+      <c r="AM8" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+    <row r="9" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>4</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1717,7 +1986,7 @@
         <v>61</v>
       </c>
       <c r="I9" s="7"/>
-      <c r="J9" s="7" t="n">
+      <c r="J9" s="7">
         <v>1</v>
       </c>
       <c r="K9" s="7"/>
@@ -1725,7 +1994,7 @@
       <c r="M9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="N9" s="10" t="n">
+      <c r="N9" s="10">
         <v>90375408</v>
       </c>
       <c r="O9" s="10"/>
@@ -1755,25 +2024,25 @@
       <c r="AE9" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF9" s="9" t="n">
-        <v>0.034</v>
+      <c r="AF9" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AG9" s="7"/>
       <c r="AH9" s="7"/>
       <c r="AI9" s="7"/>
-      <c r="AJ9" s="7" t="n">
+      <c r="AJ9" s="7">
         <v>3</v>
       </c>
-      <c r="AK9" s="7" t="n">
+      <c r="AK9" s="7">
         <v>4</v>
       </c>
       <c r="AL9" s="7"/>
-      <c r="AM9" s="7" t="n">
+      <c r="AM9" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>5</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -1798,7 +2067,7 @@
         <v>61</v>
       </c>
       <c r="I10" s="7"/>
-      <c r="J10" s="7" t="n">
+      <c r="J10" s="7">
         <v>1</v>
       </c>
       <c r="K10" s="7"/>
@@ -1806,7 +2075,7 @@
       <c r="M10" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="N10" s="10" t="n">
+      <c r="N10" s="10">
         <v>40822549</v>
       </c>
       <c r="O10" s="10"/>
@@ -1836,25 +2105,25 @@
       <c r="AE10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF10" s="9" t="n">
-        <v>0.034</v>
+      <c r="AF10" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AG10" s="7"/>
       <c r="AH10" s="7"/>
       <c r="AI10" s="7"/>
-      <c r="AJ10" s="7" t="n">
+      <c r="AJ10" s="7">
         <v>3</v>
       </c>
-      <c r="AK10" s="7" t="n">
+      <c r="AK10" s="7">
         <v>5</v>
       </c>
       <c r="AL10" s="7"/>
-      <c r="AM10" s="7" t="n">
+      <c r="AM10" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+    <row r="11" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -1879,7 +2148,7 @@
         <v>61</v>
       </c>
       <c r="I11" s="7"/>
-      <c r="J11" s="7" t="n">
+      <c r="J11" s="7">
         <v>1</v>
       </c>
       <c r="K11" s="7"/>
@@ -1887,7 +2156,7 @@
       <c r="M11" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="N11" s="10" t="n">
+      <c r="N11" s="10">
         <v>42357278</v>
       </c>
       <c r="O11" s="10"/>
@@ -1917,25 +2186,25 @@
       <c r="AE11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF11" s="9" t="n">
-        <v>0.034</v>
+      <c r="AF11" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AG11" s="7"/>
       <c r="AH11" s="7"/>
       <c r="AI11" s="7"/>
-      <c r="AJ11" s="7" t="n">
+      <c r="AJ11" s="7">
         <v>3</v>
       </c>
-      <c r="AK11" s="7" t="n">
+      <c r="AK11" s="7">
         <v>6</v>
       </c>
       <c r="AL11" s="7"/>
-      <c r="AM11" s="7" t="n">
+      <c r="AM11" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+    <row r="12" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
         <v>7</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -1960,7 +2229,7 @@
         <v>61</v>
       </c>
       <c r="I12" s="7"/>
-      <c r="J12" s="7" t="n">
+      <c r="J12" s="7">
         <v>1</v>
       </c>
       <c r="K12" s="7"/>
@@ -1968,7 +2237,7 @@
       <c r="M12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="N12" s="16" t="n">
+      <c r="N12" s="16">
         <v>42357285</v>
       </c>
       <c r="O12" s="10"/>
@@ -1998,25 +2267,25 @@
       <c r="AE12" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF12" s="9" t="n">
-        <v>0.034</v>
+      <c r="AF12" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AG12" s="7"/>
       <c r="AH12" s="7"/>
       <c r="AI12" s="7"/>
-      <c r="AJ12" s="7" t="n">
+      <c r="AJ12" s="7">
         <v>3</v>
       </c>
-      <c r="AK12" s="7" t="n">
+      <c r="AK12" s="7">
         <v>7</v>
       </c>
       <c r="AL12" s="7"/>
-      <c r="AM12" s="7" t="n">
+      <c r="AM12" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+    <row r="13" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -2041,7 +2310,7 @@
         <v>61</v>
       </c>
       <c r="I13" s="7"/>
-      <c r="J13" s="7" t="n">
+      <c r="J13" s="7">
         <v>1</v>
       </c>
       <c r="K13" s="7"/>
@@ -2079,25 +2348,25 @@
       <c r="AE13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF13" s="9" t="n">
-        <v>0.034</v>
+      <c r="AF13" s="9">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AG13" s="7"/>
       <c r="AH13" s="7"/>
       <c r="AI13" s="7"/>
-      <c r="AJ13" s="7" t="n">
+      <c r="AJ13" s="7">
         <v>3</v>
       </c>
-      <c r="AK13" s="7" t="n">
+      <c r="AK13" s="7">
         <v>8</v>
       </c>
       <c r="AL13" s="7"/>
-      <c r="AM13" s="7" t="n">
+      <c r="AM13" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+    <row r="14" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -2152,21 +2421,21 @@
       <c r="AG14" s="7"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
-      <c r="AJ14" s="7" t="n">
+      <c r="AJ14" s="7">
         <v>2</v>
       </c>
-      <c r="AK14" s="7" t="n">
+      <c r="AK14" s="7">
         <v>9</v>
       </c>
-      <c r="AL14" s="7" t="n">
+      <c r="AL14" s="7">
         <v>10</v>
       </c>
-      <c r="AM14" s="13" t="n">
+      <c r="AM14" s="13">
         <v>300</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+    <row r="15" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
         <v>10</v>
       </c>
       <c r="B15" s="7" t="s">
@@ -2191,7 +2460,7 @@
         <v>61</v>
       </c>
       <c r="I15" s="7"/>
-      <c r="J15" s="7" t="n">
+      <c r="J15" s="7">
         <v>1</v>
       </c>
       <c r="K15" s="7"/>
@@ -2229,25 +2498,25 @@
       <c r="AE15" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF15" s="9" t="n">
+      <c r="AF15" s="9">
         <v>0.05</v>
       </c>
       <c r="AG15" s="18"/>
       <c r="AH15" s="7"/>
       <c r="AI15" s="7"/>
-      <c r="AJ15" s="7" t="n">
+      <c r="AJ15" s="7">
         <v>3</v>
       </c>
-      <c r="AK15" s="7" t="n">
+      <c r="AK15" s="7">
         <v>10</v>
       </c>
       <c r="AL15" s="7"/>
-      <c r="AM15" s="7" t="n">
+      <c r="AM15" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
+    <row r="16" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
         <v>11</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2302,21 +2571,21 @@
       <c r="AG16" s="7"/>
       <c r="AH16" s="7"/>
       <c r="AI16" s="7"/>
-      <c r="AJ16" s="7" t="n">
+      <c r="AJ16" s="7">
         <v>2</v>
       </c>
-      <c r="AK16" s="7" t="n">
+      <c r="AK16" s="7">
         <v>11</v>
       </c>
       <c r="AL16" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="AM16" s="13" t="n">
+      <c r="AM16" s="13">
         <v>300</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
+    <row r="17" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
         <v>12</v>
       </c>
       <c r="B17" s="7" t="s">
@@ -2341,7 +2610,7 @@
         <v>61</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="7" t="n">
+      <c r="J17" s="7">
         <v>1</v>
       </c>
       <c r="K17" s="7"/>
@@ -2349,7 +2618,7 @@
       <c r="M17" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="N17" s="10" t="n">
+      <c r="N17" s="10">
         <v>4650075420386</v>
       </c>
       <c r="O17" s="10"/>
@@ -2379,25 +2648,25 @@
       <c r="AE17" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF17" s="9" t="n">
+      <c r="AF17" s="9">
         <v>0.05</v>
       </c>
       <c r="AG17" s="7"/>
       <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
-      <c r="AJ17" s="7" t="n">
+      <c r="AJ17" s="7">
         <v>3</v>
       </c>
-      <c r="AK17" s="7" t="n">
+      <c r="AK17" s="7">
         <v>12</v>
       </c>
       <c r="AL17" s="7"/>
-      <c r="AM17" s="7" t="n">
+      <c r="AM17" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+    <row r="18" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
         <v>13</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -2422,7 +2691,7 @@
         <v>61</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="7" t="n">
+      <c r="J18" s="7">
         <v>1</v>
       </c>
       <c r="K18" s="7"/>
@@ -2430,7 +2699,7 @@
       <c r="M18" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="N18" s="10" t="n">
+      <c r="N18" s="10">
         <v>4650075420362</v>
       </c>
       <c r="O18" s="10"/>
@@ -2460,25 +2729,25 @@
       <c r="AE18" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF18" s="9" t="n">
-        <v>0.036667</v>
+      <c r="AF18" s="9">
+        <v>3.6666999999999998E-2</v>
       </c>
       <c r="AG18" s="7"/>
       <c r="AH18" s="7"/>
       <c r="AI18" s="7"/>
-      <c r="AJ18" s="7" t="n">
+      <c r="AJ18" s="7">
         <v>3</v>
       </c>
-      <c r="AK18" s="7" t="n">
+      <c r="AK18" s="7">
         <v>13</v>
       </c>
       <c r="AL18" s="7"/>
-      <c r="AM18" s="7" t="n">
+      <c r="AM18" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+    <row r="19" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
         <v>14</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -2503,7 +2772,7 @@
         <v>97</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="7" t="n">
+      <c r="J19" s="7">
         <v>1</v>
       </c>
       <c r="K19" s="7"/>
@@ -2533,27 +2802,27 @@
       <c r="AE19" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF19" s="9" t="n">
+      <c r="AF19" s="9">
         <v>0.02</v>
       </c>
       <c r="AG19" s="7"/>
       <c r="AH19" s="7"/>
       <c r="AI19" s="7"/>
-      <c r="AJ19" s="7" t="n">
+      <c r="AJ19" s="7">
         <v>3</v>
       </c>
-      <c r="AK19" s="7" t="n">
+      <c r="AK19" s="7">
         <v>14</v>
       </c>
       <c r="AL19" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AM19" s="7" t="n">
+      <c r="AM19" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+    <row r="20" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
         <v>15</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2578,7 +2847,7 @@
         <v>61</v>
       </c>
       <c r="I20" s="7"/>
-      <c r="J20" s="7" t="n">
+      <c r="J20" s="7">
         <v>1</v>
       </c>
       <c r="K20" s="7"/>
@@ -2586,7 +2855,7 @@
       <c r="M20" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="10" t="n">
+      <c r="N20" s="10">
         <v>4650075420508</v>
       </c>
       <c r="O20" s="10"/>
@@ -2620,19 +2889,19 @@
       <c r="AG20" s="7"/>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
-      <c r="AJ20" s="7" t="n">
+      <c r="AJ20" s="7">
         <v>4</v>
       </c>
-      <c r="AK20" s="7" t="n">
+      <c r="AK20" s="7">
         <v>15</v>
       </c>
       <c r="AL20" s="7"/>
-      <c r="AM20" s="7" t="n">
+      <c r="AM20" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+    <row r="21" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
         <v>16</v>
       </c>
       <c r="B21" s="7" t="s">
@@ -2657,7 +2926,7 @@
         <v>61</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="7" t="n">
+      <c r="J21" s="7">
         <v>1</v>
       </c>
       <c r="K21" s="7"/>
@@ -2665,7 +2934,7 @@
       <c r="M21" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="N21" s="10" t="n">
+      <c r="N21" s="10">
         <v>4650075420423</v>
       </c>
       <c r="O21" s="10"/>
@@ -2699,19 +2968,19 @@
       <c r="AG21" s="7"/>
       <c r="AH21" s="7"/>
       <c r="AI21" s="7"/>
-      <c r="AJ21" s="7" t="n">
+      <c r="AJ21" s="7">
         <v>4</v>
       </c>
-      <c r="AK21" s="7" t="n">
+      <c r="AK21" s="7">
         <v>16</v>
       </c>
       <c r="AL21" s="7"/>
-      <c r="AM21" s="7" t="n">
+      <c r="AM21" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+    <row r="22" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
         <v>17</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -2736,7 +3005,7 @@
         <v>61</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="7" t="n">
+      <c r="J22" s="7">
         <v>1</v>
       </c>
       <c r="K22" s="7"/>
@@ -2744,7 +3013,7 @@
       <c r="M22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="N22" s="10" t="n">
+      <c r="N22" s="10">
         <v>4650075420485</v>
       </c>
       <c r="O22" s="10"/>
@@ -2778,19 +3047,19 @@
       <c r="AG22" s="7"/>
       <c r="AH22" s="7"/>
       <c r="AI22" s="7"/>
-      <c r="AJ22" s="7" t="n">
+      <c r="AJ22" s="7">
         <v>4</v>
       </c>
-      <c r="AK22" s="7" t="n">
+      <c r="AK22" s="7">
         <v>17</v>
       </c>
       <c r="AL22" s="7"/>
-      <c r="AM22" s="7" t="n">
+      <c r="AM22" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+    <row r="23" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>18</v>
       </c>
       <c r="B23" s="7" t="s">
@@ -2815,7 +3084,7 @@
         <v>61</v>
       </c>
       <c r="I23" s="7"/>
-      <c r="J23" s="7" t="n">
+      <c r="J23" s="7">
         <v>1</v>
       </c>
       <c r="K23" s="7"/>
@@ -2823,7 +3092,7 @@
       <c r="M23" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="N23" s="10" t="n">
+      <c r="N23" s="10">
         <v>4650075420447</v>
       </c>
       <c r="O23" s="10"/>
@@ -2857,19 +3126,19 @@
       <c r="AG23" s="7"/>
       <c r="AH23" s="7"/>
       <c r="AI23" s="7"/>
-      <c r="AJ23" s="7" t="n">
+      <c r="AJ23" s="7">
         <v>4</v>
       </c>
-      <c r="AK23" s="7" t="n">
+      <c r="AK23" s="7">
         <v>18</v>
       </c>
       <c r="AL23" s="7"/>
-      <c r="AM23" s="7" t="n">
+      <c r="AM23" s="7">
         <v>14</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+    <row r="24" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
         <v>19</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -2894,7 +3163,7 @@
         <v>61</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="7" t="n">
+      <c r="J24" s="7">
         <v>1</v>
       </c>
       <c r="K24" s="7"/>
@@ -2902,7 +3171,7 @@
       <c r="M24" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="N24" s="10" t="n">
+      <c r="N24" s="10">
         <v>4650075420409</v>
       </c>
       <c r="O24" s="10"/>
@@ -2932,25 +3201,25 @@
       <c r="AE24" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF24" s="9" t="n">
-        <v>0.036667</v>
+      <c r="AF24" s="9">
+        <v>3.6666999999999998E-2</v>
       </c>
       <c r="AG24" s="7"/>
       <c r="AH24" s="7"/>
       <c r="AI24" s="7"/>
-      <c r="AJ24" s="7" t="n">
+      <c r="AJ24" s="7">
         <v>3</v>
       </c>
-      <c r="AK24" s="7" t="n">
+      <c r="AK24" s="7">
         <v>19</v>
       </c>
       <c r="AL24" s="7"/>
-      <c r="AM24" s="7" t="n">
+      <c r="AM24" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+    <row r="25" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
         <v>20</v>
       </c>
       <c r="B25" s="7" t="s">
@@ -3005,21 +3274,21 @@
       <c r="AG25" s="7"/>
       <c r="AH25" s="7"/>
       <c r="AI25" s="7"/>
-      <c r="AJ25" s="7" t="n">
+      <c r="AJ25" s="7">
         <v>2</v>
       </c>
-      <c r="AK25" s="7" t="n">
+      <c r="AK25" s="7">
         <v>20</v>
       </c>
-      <c r="AL25" s="7" t="n">
+      <c r="AL25" s="7">
         <v>21</v>
       </c>
-      <c r="AM25" s="13" t="n">
+      <c r="AM25" s="13">
         <v>300</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+    <row r="26" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
         <v>21</v>
       </c>
       <c r="B26" s="7" t="s">
@@ -3044,7 +3313,7 @@
         <v>61</v>
       </c>
       <c r="I26" s="7"/>
-      <c r="J26" s="7" t="n">
+      <c r="J26" s="7">
         <v>1</v>
       </c>
       <c r="K26" s="7"/>
@@ -3086,25 +3355,25 @@
       <c r="AE26" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF26" s="9" t="n">
-        <v>0.036667</v>
+      <c r="AF26" s="9">
+        <v>3.6666999999999998E-2</v>
       </c>
       <c r="AG26" s="7"/>
       <c r="AH26" s="7"/>
       <c r="AI26" s="7"/>
-      <c r="AJ26" s="7" t="n">
+      <c r="AJ26" s="7">
         <v>3</v>
       </c>
-      <c r="AK26" s="7" t="n">
+      <c r="AK26" s="7">
         <v>21</v>
       </c>
       <c r="AL26" s="7"/>
-      <c r="AM26" s="7" t="n">
+      <c r="AM26" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+    <row r="27" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
         <v>22</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -3129,7 +3398,7 @@
         <v>61</v>
       </c>
       <c r="I27" s="7"/>
-      <c r="J27" s="7" t="n">
+      <c r="J27" s="7">
         <v>1</v>
       </c>
       <c r="K27" s="7"/>
@@ -3167,25 +3436,25 @@
       <c r="AE27" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF27" s="9" t="n">
-        <v>0.166667</v>
+      <c r="AF27" s="9">
+        <v>0.16666700000000001</v>
       </c>
       <c r="AG27" s="18"/>
       <c r="AH27" s="20"/>
       <c r="AI27" s="7"/>
-      <c r="AJ27" s="7" t="n">
+      <c r="AJ27" s="7">
         <v>2</v>
       </c>
-      <c r="AK27" s="7" t="n">
+      <c r="AK27" s="7">
         <v>22</v>
       </c>
       <c r="AL27" s="7"/>
-      <c r="AM27" s="13" t="n">
+      <c r="AM27" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+    <row r="28" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
         <v>23</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3210,7 +3479,7 @@
         <v>127</v>
       </c>
       <c r="I28" s="7"/>
-      <c r="J28" s="7" t="n">
+      <c r="J28" s="7">
         <v>1</v>
       </c>
       <c r="K28" s="7"/>
@@ -3242,27 +3511,27 @@
       <c r="AE28" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF28" s="9" t="n">
-        <v>0.083333</v>
+      <c r="AF28" s="9">
+        <v>8.3333000000000004E-2</v>
       </c>
       <c r="AG28" s="18"/>
       <c r="AH28" s="7"/>
       <c r="AI28" s="7"/>
-      <c r="AJ28" s="7" t="n">
+      <c r="AJ28" s="7">
         <v>2</v>
       </c>
-      <c r="AK28" s="7" t="n">
+      <c r="AK28" s="7">
         <v>23</v>
       </c>
-      <c r="AL28" s="7" t="n">
+      <c r="AL28" s="7">
         <v>24</v>
       </c>
-      <c r="AM28" s="13" t="n">
+      <c r="AM28" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
+    <row r="29" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
         <v>24</v>
       </c>
       <c r="B29" s="7" t="s">
@@ -3287,7 +3556,7 @@
         <v>61</v>
       </c>
       <c r="I29" s="7"/>
-      <c r="J29" s="7" t="n">
+      <c r="J29" s="7">
         <v>3</v>
       </c>
       <c r="K29" s="7"/>
@@ -3333,19 +3602,19 @@
       <c r="AG29" s="18"/>
       <c r="AH29" s="7"/>
       <c r="AI29" s="7"/>
-      <c r="AJ29" s="7" t="n">
+      <c r="AJ29" s="7">
         <v>3</v>
       </c>
-      <c r="AK29" s="7" t="n">
+      <c r="AK29" s="7">
         <v>24</v>
       </c>
       <c r="AL29" s="7"/>
-      <c r="AM29" s="7" t="n">
+      <c r="AM29" s="7">
         <v>23</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
+    <row r="30" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="7">
         <v>25</v>
       </c>
       <c r="B30" s="7" t="s">
@@ -3370,7 +3639,7 @@
         <v>127</v>
       </c>
       <c r="I30" s="7"/>
-      <c r="J30" s="7" t="n">
+      <c r="J30" s="7">
         <v>1</v>
       </c>
       <c r="K30" s="7"/>
@@ -3402,27 +3671,27 @@
       <c r="AE30" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF30" s="9" t="n">
-        <v>0.083333</v>
+      <c r="AF30" s="9">
+        <v>8.3333000000000004E-2</v>
       </c>
       <c r="AG30" s="18"/>
       <c r="AH30" s="7"/>
       <c r="AI30" s="7"/>
-      <c r="AJ30" s="7" t="n">
+      <c r="AJ30" s="7">
         <v>2</v>
       </c>
-      <c r="AK30" s="7" t="n">
+      <c r="AK30" s="7">
         <v>25</v>
       </c>
       <c r="AL30" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="AM30" s="13" t="n">
+      <c r="AM30" s="13">
         <v>400</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+    <row r="31" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7">
         <v>26</v>
       </c>
       <c r="B31" s="7" t="s">
@@ -3447,7 +3716,7 @@
         <v>61</v>
       </c>
       <c r="I31" s="7"/>
-      <c r="J31" s="7" t="n">
+      <c r="J31" s="7">
         <v>1</v>
       </c>
       <c r="K31" s="7"/>
@@ -3489,19 +3758,19 @@
       <c r="AG31" s="18"/>
       <c r="AH31" s="7"/>
       <c r="AI31" s="7"/>
-      <c r="AJ31" s="7" t="n">
+      <c r="AJ31" s="7">
         <v>3</v>
       </c>
-      <c r="AK31" s="7" t="n">
+      <c r="AK31" s="7">
         <v>26</v>
       </c>
       <c r="AL31" s="7"/>
-      <c r="AM31" s="7" t="n">
+      <c r="AM31" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
+    <row r="32" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3526,7 +3795,7 @@
         <v>61</v>
       </c>
       <c r="I32" s="7"/>
-      <c r="J32" s="7" t="n">
+      <c r="J32" s="7">
         <v>1</v>
       </c>
       <c r="K32" s="7"/>
@@ -3570,19 +3839,19 @@
       <c r="AG32" s="18"/>
       <c r="AH32" s="7"/>
       <c r="AI32" s="7"/>
-      <c r="AJ32" s="7" t="n">
+      <c r="AJ32" s="7">
         <v>3</v>
       </c>
-      <c r="AK32" s="7" t="n">
+      <c r="AK32" s="7">
         <v>27</v>
       </c>
       <c r="AL32" s="7"/>
-      <c r="AM32" s="7" t="n">
+      <c r="AM32" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+    <row r="33" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
         <v>28</v>
       </c>
       <c r="B33" s="7" t="s">
@@ -3607,7 +3876,7 @@
         <v>127</v>
       </c>
       <c r="I33" s="7"/>
-      <c r="J33" s="7" t="n">
+      <c r="J33" s="7">
         <v>1</v>
       </c>
       <c r="K33" s="7"/>
@@ -3635,27 +3904,27 @@
       <c r="AE33" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="AF33" s="9" t="n">
+      <c r="AF33" s="9">
         <v>0.12</v>
       </c>
       <c r="AG33" s="7"/>
       <c r="AH33" s="7"/>
       <c r="AI33" s="7"/>
-      <c r="AJ33" s="22" t="n">
+      <c r="AJ33" s="22">
         <v>2</v>
       </c>
-      <c r="AK33" s="7" t="n">
+      <c r="AK33" s="7">
         <v>29</v>
       </c>
       <c r="AL33" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="AM33" s="7" t="n">
+      <c r="AM33" s="7">
         <v>400</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="n">
+    <row r="34" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
         <v>29</v>
       </c>
       <c r="B34" s="7" t="s">
@@ -3680,7 +3949,7 @@
         <v>61</v>
       </c>
       <c r="I34" s="24"/>
-      <c r="J34" s="22" t="n">
+      <c r="J34" s="22">
         <v>1</v>
       </c>
       <c r="K34" s="24"/>
@@ -3722,19 +3991,19 @@
       <c r="AG34" s="24"/>
       <c r="AH34" s="24"/>
       <c r="AI34" s="24"/>
-      <c r="AJ34" s="22" t="n">
+      <c r="AJ34" s="22">
         <v>3</v>
       </c>
-      <c r="AK34" s="22" t="n">
+      <c r="AK34" s="22">
         <v>900</v>
       </c>
       <c r="AL34" s="22"/>
-      <c r="AM34" s="22" t="n">
+      <c r="AM34" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="n">
+    <row r="35" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
         <v>30</v>
       </c>
       <c r="B35" s="7" t="s">
@@ -3759,7 +4028,7 @@
         <v>97</v>
       </c>
       <c r="I35" s="24"/>
-      <c r="J35" s="22" t="n">
+      <c r="J35" s="22">
         <v>2</v>
       </c>
       <c r="K35" s="24"/>
@@ -3793,21 +4062,21 @@
       <c r="AG35" s="24"/>
       <c r="AH35" s="24"/>
       <c r="AI35" s="24"/>
-      <c r="AJ35" s="22" t="n">
+      <c r="AJ35" s="22">
         <v>3</v>
       </c>
-      <c r="AK35" s="22" t="n">
+      <c r="AK35" s="22">
         <v>901</v>
       </c>
       <c r="AL35" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="AM35" s="22" t="n">
+      <c r="AM35" s="22">
         <v>29</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="n">
+    <row r="36" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="7">
         <v>31</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -3832,7 +4101,7 @@
         <v>61</v>
       </c>
       <c r="I36" s="24"/>
-      <c r="J36" s="22" t="n">
+      <c r="J36" s="22">
         <v>1</v>
       </c>
       <c r="K36" s="24"/>
@@ -3874,19 +4143,19 @@
       <c r="AG36" s="24"/>
       <c r="AH36" s="24"/>
       <c r="AI36" s="24"/>
-      <c r="AJ36" s="22" t="n">
+      <c r="AJ36" s="22">
         <v>4</v>
       </c>
-      <c r="AK36" s="22" t="n">
+      <c r="AK36" s="22">
         <v>902</v>
       </c>
       <c r="AL36" s="22"/>
-      <c r="AM36" s="22" t="n">
+      <c r="AM36" s="22">
         <v>901</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="n">
+    <row r="37" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7">
         <v>32</v>
       </c>
       <c r="B37" s="7" t="s">
@@ -3911,7 +4180,7 @@
         <v>61</v>
       </c>
       <c r="I37" s="24"/>
-      <c r="J37" s="22" t="n">
+      <c r="J37" s="22">
         <v>1</v>
       </c>
       <c r="K37" s="24"/>
@@ -3919,7 +4188,7 @@
       <c r="M37" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="N37" s="7" t="n">
+      <c r="N37" s="7">
         <v>5000034</v>
       </c>
       <c r="O37" s="7"/>
@@ -3951,19 +4220,19 @@
       <c r="AG37" s="24"/>
       <c r="AH37" s="24"/>
       <c r="AI37" s="24"/>
-      <c r="AJ37" s="22" t="n">
+      <c r="AJ37" s="22">
         <v>4</v>
       </c>
-      <c r="AK37" s="22" t="n">
+      <c r="AK37" s="22">
         <v>903</v>
       </c>
       <c r="AL37" s="22"/>
-      <c r="AM37" s="22" t="n">
+      <c r="AM37" s="22">
         <v>901</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="n">
+    <row r="38" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
         <v>33</v>
       </c>
       <c r="B38" s="7" t="s">
@@ -3988,7 +4257,7 @@
         <v>127</v>
       </c>
       <c r="I38" s="7"/>
-      <c r="J38" s="7" t="n">
+      <c r="J38" s="7">
         <v>3</v>
       </c>
       <c r="K38" s="7"/>
@@ -4018,27 +4287,27 @@
       <c r="AE38" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="AF38" s="9" t="n">
-        <v>0.046666</v>
+      <c r="AF38" s="9">
+        <v>4.6665999999999999E-2</v>
       </c>
       <c r="AG38" s="7"/>
       <c r="AH38" s="7"/>
       <c r="AI38" s="7"/>
-      <c r="AJ38" s="7" t="n">
+      <c r="AJ38" s="7">
         <v>2</v>
       </c>
-      <c r="AK38" s="7" t="n">
+      <c r="AK38" s="7">
         <v>33</v>
       </c>
       <c r="AL38" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="AM38" s="13" t="n">
+      <c r="AM38" s="13">
         <v>312</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="n">
+    <row r="39" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
         <v>34</v>
       </c>
       <c r="B39" s="7" t="s">
@@ -4063,7 +4332,7 @@
         <v>171</v>
       </c>
       <c r="I39" s="7"/>
-      <c r="J39" s="7" t="n">
+      <c r="J39" s="7">
         <v>1</v>
       </c>
       <c r="K39" s="7"/>
@@ -4101,19 +4370,19 @@
       <c r="AG39" s="7"/>
       <c r="AH39" s="7"/>
       <c r="AI39" s="7"/>
-      <c r="AJ39" s="7" t="n">
+      <c r="AJ39" s="7">
         <v>3</v>
       </c>
-      <c r="AK39" s="7" t="n">
+      <c r="AK39" s="7">
         <v>34</v>
       </c>
       <c r="AL39" s="7"/>
-      <c r="AM39" s="7" t="n">
+      <c r="AM39" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="n">
+    <row r="40" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7">
         <v>35</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -4138,7 +4407,7 @@
         <v>176</v>
       </c>
       <c r="I40" s="7"/>
-      <c r="J40" s="7" t="n">
+      <c r="J40" s="7">
         <v>1</v>
       </c>
       <c r="K40" s="7"/>
@@ -4180,19 +4449,19 @@
       <c r="AI40" s="7" t="s">
         <v>178</v>
       </c>
-      <c r="AJ40" s="7" t="n">
+      <c r="AJ40" s="7">
         <v>3</v>
       </c>
-      <c r="AK40" s="7" t="n">
+      <c r="AK40" s="7">
         <v>35</v>
       </c>
       <c r="AL40" s="7"/>
-      <c r="AM40" s="7" t="n">
+      <c r="AM40" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="n">
+    <row r="41" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="7">
         <v>36</v>
       </c>
       <c r="B41" s="7" t="s">
@@ -4217,7 +4486,7 @@
         <v>181</v>
       </c>
       <c r="I41" s="7"/>
-      <c r="J41" s="7" t="n">
+      <c r="J41" s="7">
         <v>1</v>
       </c>
       <c r="K41" s="7"/>
@@ -4259,19 +4528,19 @@
       <c r="AI41" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="AJ41" s="7" t="n">
+      <c r="AJ41" s="7">
         <v>3</v>
       </c>
-      <c r="AK41" s="7" t="n">
+      <c r="AK41" s="7">
         <v>36</v>
       </c>
       <c r="AL41" s="7"/>
-      <c r="AM41" s="7" t="n">
+      <c r="AM41" s="7">
         <v>33</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="n">
+    <row r="42" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
         <v>37</v>
       </c>
       <c r="B42" s="7" t="s">
@@ -4284,7 +4553,7 @@
         <v>183</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>164</v>
+        <v>206</v>
       </c>
       <c r="F42" s="21" t="s">
         <v>184</v>
@@ -4293,10 +4562,10 @@
         <v>185</v>
       </c>
       <c r="H42" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="I42" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="I42" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
@@ -4309,7 +4578,7 @@
       <c r="R42" s="7"/>
       <c r="S42" s="7"/>
       <c r="T42" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U42" s="7"/>
       <c r="V42" s="7"/>
@@ -4327,16 +4596,16 @@
       <c r="AH42" s="7"/>
       <c r="AI42" s="7"/>
       <c r="AJ42" s="7"/>
-      <c r="AK42" s="7" t="n">
+      <c r="AK42" s="7">
         <v>38</v>
       </c>
-      <c r="AL42" s="7" t="n">
-        <v>33</v>
+      <c r="AL42" s="12" t="s">
+        <v>208</v>
       </c>
       <c r="AM42" s="7"/>
     </row>
-    <row r="43" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="n">
+    <row r="43" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7">
         <v>38</v>
       </c>
       <c r="B43" s="7" t="s">
@@ -4352,23 +4621,23 @@
         <v>117</v>
       </c>
       <c r="F43" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="H43" s="7" t="s">
         <v>190</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="I43" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I43" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
       <c r="N43" s="12" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
@@ -4376,7 +4645,7 @@
       <c r="R43" s="7"/>
       <c r="S43" s="7"/>
       <c r="T43" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U43" s="7"/>
       <c r="V43" s="7"/>
@@ -4394,16 +4663,16 @@
       <c r="AH43" s="7"/>
       <c r="AI43" s="7"/>
       <c r="AJ43" s="7"/>
-      <c r="AK43" s="7" t="n">
+      <c r="AK43" s="7">
         <v>39</v>
       </c>
-      <c r="AL43" s="7" t="n">
+      <c r="AL43" s="7">
         <v>22</v>
       </c>
       <c r="AM43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="n">
+    <row r="44" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -4419,23 +4688,23 @@
         <v>124</v>
       </c>
       <c r="F44" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="H44" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I44" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I44" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
       <c r="L44" s="7"/>
       <c r="M44" s="7"/>
       <c r="N44" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
@@ -4443,7 +4712,7 @@
       <c r="R44" s="7"/>
       <c r="S44" s="7"/>
       <c r="T44" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U44" s="7"/>
       <c r="V44" s="7"/>
@@ -4461,16 +4730,16 @@
       <c r="AH44" s="7"/>
       <c r="AI44" s="7"/>
       <c r="AJ44" s="7"/>
-      <c r="AK44" s="7" t="n">
+      <c r="AK44" s="7">
         <v>40</v>
       </c>
-      <c r="AL44" s="7" t="n">
+      <c r="AL44" s="7">
         <v>23</v>
       </c>
       <c r="AM44" s="7"/>
     </row>
-    <row r="45" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="n">
+    <row r="45" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
         <v>40</v>
       </c>
       <c r="B45" s="7" t="s">
@@ -4486,23 +4755,23 @@
         <v>124</v>
       </c>
       <c r="F45" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="G45" s="7" t="s">
-        <v>195</v>
-      </c>
       <c r="H45" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I45" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I45" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
       <c r="L45" s="7"/>
       <c r="M45" s="7"/>
       <c r="N45" s="12" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
@@ -4510,7 +4779,7 @@
       <c r="R45" s="7"/>
       <c r="S45" s="7"/>
       <c r="T45" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U45" s="7"/>
       <c r="V45" s="7"/>
@@ -4528,16 +4797,16 @@
       <c r="AH45" s="7"/>
       <c r="AI45" s="7"/>
       <c r="AJ45" s="7"/>
-      <c r="AK45" s="7" t="n">
+      <c r="AK45" s="7">
         <v>41</v>
       </c>
-      <c r="AL45" s="7" t="n">
+      <c r="AL45" s="7">
         <v>25</v>
       </c>
       <c r="AM45" s="7"/>
     </row>
-    <row r="46" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="n">
+    <row r="46" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
         <v>41</v>
       </c>
       <c r="B46" s="7" t="s">
@@ -4550,26 +4819,28 @@
         <v>183</v>
       </c>
       <c r="E46" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G46" s="21" t="s">
         <v>198</v>
       </c>
-      <c r="F46" s="21" t="s">
-        <v>199</v>
-      </c>
-      <c r="G46" s="21" t="s">
-        <v>200</v>
-      </c>
       <c r="H46" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I46" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I46" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
-      <c r="M46" s="7"/>
+      <c r="M46" s="30" t="s">
+        <v>210</v>
+      </c>
       <c r="N46" s="12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
@@ -4577,7 +4848,7 @@
       <c r="R46" s="7"/>
       <c r="S46" s="7"/>
       <c r="T46" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U46" s="7"/>
       <c r="V46" s="7"/>
@@ -4595,17 +4866,17 @@
       <c r="AH46" s="7"/>
       <c r="AI46" s="7"/>
       <c r="AJ46" s="7"/>
-      <c r="AK46" s="7" t="n">
+      <c r="AK46" s="7">
         <v>42</v>
       </c>
-      <c r="AL46" s="7" t="n">
-        <v>32</v>
+      <c r="AL46" s="7">
+        <v>29</v>
       </c>
       <c r="AM46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="n">
-        <v>42</v>
+    <row r="47" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="7">
+        <v>43</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>39</v>
@@ -4616,27 +4887,27 @@
       <c r="D47" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E47" s="21" t="s">
-        <v>198</v>
+      <c r="E47" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="F47" s="21" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G47" s="21" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H47" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I47" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I47" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
       <c r="L47" s="7"/>
       <c r="M47" s="7"/>
-      <c r="N47" s="12" t="s">
-        <v>202</v>
+      <c r="N47" s="31" t="s">
+        <v>211</v>
       </c>
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
@@ -4644,7 +4915,7 @@
       <c r="R47" s="7"/>
       <c r="S47" s="7"/>
       <c r="T47" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U47" s="7"/>
       <c r="V47" s="7"/>
@@ -4662,17 +4933,17 @@
       <c r="AH47" s="7"/>
       <c r="AI47" s="7"/>
       <c r="AJ47" s="7"/>
-      <c r="AK47" s="7" t="n">
-        <v>43</v>
-      </c>
-      <c r="AL47" s="7" t="n">
-        <v>29</v>
+      <c r="AK47" s="7">
+        <v>44</v>
+      </c>
+      <c r="AL47" s="12" t="s">
+        <v>212</v>
       </c>
       <c r="AM47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="n">
-        <v>43</v>
+    <row r="48" spans="1:39" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="7">
+        <v>44</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>39</v>
@@ -4684,26 +4955,28 @@
         <v>183</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G48" s="21" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="H48" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="I48" s="7" t="s">
         <v>191</v>
-      </c>
-      <c r="I48" s="7" t="s">
-        <v>192</v>
       </c>
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
       <c r="L48" s="7"/>
-      <c r="M48" s="7"/>
-      <c r="N48" s="12" t="s">
-        <v>206</v>
+      <c r="M48" s="30" t="s">
+        <v>210</v>
+      </c>
+      <c r="N48" s="31" t="s">
+        <v>213</v>
       </c>
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
@@ -4711,7 +4984,7 @@
       <c r="R48" s="7"/>
       <c r="S48" s="7"/>
       <c r="T48" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U48" s="7"/>
       <c r="V48" s="7"/>
@@ -4729,17 +5002,17 @@
       <c r="AH48" s="7"/>
       <c r="AI48" s="7"/>
       <c r="AJ48" s="7"/>
-      <c r="AK48" s="7" t="n">
-        <v>44</v>
+      <c r="AK48" s="7">
+        <v>45</v>
       </c>
       <c r="AL48" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="AM48" s="7"/>
     </row>
-    <row r="49" customFormat="false" ht="22.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="n">
-        <v>44</v>
+    <row r="49" spans="1:1024" s="29" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7">
+        <v>904</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>39</v>
@@ -4750,35 +5023,31 @@
       <c r="D49" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="21"/>
+      <c r="F49" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="F49" s="21" t="s">
+      <c r="G49" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="G49" s="21" t="s">
+      <c r="H49" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="I49" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H49" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="I49" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="J49" s="7"/>
-      <c r="K49" s="7"/>
-      <c r="L49" s="7"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
       <c r="M49" s="7"/>
-      <c r="N49" s="12" t="s">
-        <v>208</v>
-      </c>
+      <c r="N49" s="27"/>
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="7"/>
       <c r="R49" s="7"/>
       <c r="S49" s="7"/>
       <c r="T49" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="U49" s="7"/>
       <c r="V49" s="7"/>
@@ -4789,92 +5058,23 @@
       <c r="AA49" s="7"/>
       <c r="AB49" s="7"/>
       <c r="AC49" s="7"/>
-      <c r="AD49" s="7"/>
+      <c r="AD49" s="28"/>
       <c r="AE49" s="7"/>
-      <c r="AF49" s="9"/>
+      <c r="AF49" s="7"/>
       <c r="AG49" s="7"/>
       <c r="AH49" s="7"/>
       <c r="AI49" s="7"/>
       <c r="AJ49" s="7"/>
-      <c r="AK49" s="7" t="n">
-        <v>45</v>
-      </c>
-      <c r="AL49" s="12" t="s">
-        <v>209</v>
-      </c>
+      <c r="AK49" s="7">
+        <v>904</v>
+      </c>
+      <c r="AL49" s="7"/>
       <c r="AM49" s="7"/>
-    </row>
-    <row r="50" s="29" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="n">
-        <v>904</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="G50" s="21" t="s">
-        <v>211</v>
-      </c>
-      <c r="H50" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="I50" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="J50" s="26"/>
-      <c r="K50" s="26"/>
-      <c r="L50" s="26"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="27"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="7"/>
-      <c r="S50" s="7"/>
-      <c r="T50" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="U50" s="7"/>
-      <c r="V50" s="7"/>
-      <c r="W50" s="7"/>
-      <c r="X50" s="7"/>
-      <c r="Y50" s="7"/>
-      <c r="Z50" s="7"/>
-      <c r="AA50" s="7"/>
-      <c r="AB50" s="7"/>
-      <c r="AC50" s="7"/>
-      <c r="AD50" s="28"/>
-      <c r="AE50" s="7"/>
-      <c r="AF50" s="7"/>
-      <c r="AG50" s="7"/>
-      <c r="AH50" s="7"/>
-      <c r="AI50" s="7"/>
-      <c r="AJ50" s="7"/>
-      <c r="AK50" s="7" t="n">
-        <v>904</v>
-      </c>
-      <c r="AL50" s="7"/>
-      <c r="AM50" s="7"/>
-      <c r="AMJ50" s="0"/>
+      <c r="AMJ49"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AM49"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <autoFilter ref="A1:AM48" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>